<commit_message>
S4Loader - work towards extracting raw PDT values with FieldEval.
</commit_message>
<xml_diff>
--- a/data/S4Loader_configs/pdt_field_eval.xlsx
+++ b/data/S4Loader_configs/pdt_field_eval.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="84">
   <si>
     <t xml:space="preserve">pdt_field_name </t>
   </si>
@@ -28,6 +28,9 @@
     <t xml:space="preserve">s4_type</t>
   </si>
   <si>
+    <t xml:space="preserve">evaluator_type</t>
+  </si>
+  <si>
     <t xml:space="preserve">evaluator</t>
   </si>
   <si>
@@ -40,7 +43,10 @@
     <t xml:space="preserve">String</t>
   </si>
   <si>
-    <t xml:space="preserve">builtin:non-empty-string</t>
+    <t xml:space="preserve">builtin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">non-empty-string</t>
   </si>
   <si>
     <t xml:space="preserve">DMP OAC 01 01 Damper-1</t>
@@ -67,7 +73,7 @@
     <t xml:space="preserve">Manufacturer</t>
   </si>
   <si>
-    <t xml:space="preserve">builtin:manufacturer</t>
+    <t xml:space="preserve">manufacturer</t>
   </si>
   <si>
     <t xml:space="preserve">Manufacturer website</t>
@@ -214,7 +220,10 @@
     <t xml:space="preserve">Decimal</t>
   </si>
   <si>
-    <t xml:space="preserve">regex:(?i)(?&lt;value&gt;\d+\.?\d*)\s?(kg)?</t>
+    <t xml:space="preserve">regex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(?i)(?&lt;value&gt;\d+\.?\d*)\s?(kg)?</t>
   </si>
   <si>
     <t xml:space="preserve">17.2 kg</t>
@@ -226,31 +235,28 @@
     <t xml:space="preserve">Manufacturer's serial number</t>
   </si>
   <si>
+    <t xml:space="preserve">any</t>
+  </si>
+  <si>
     <t xml:space="preserve">Date of installation</t>
   </si>
   <si>
     <t xml:space="preserve">Date</t>
   </si>
   <si>
-    <t xml:space="preserve">builtin:local-date</t>
+    <t xml:space="preserve">Local-date</t>
   </si>
   <si>
     <t xml:space="preserve">Tag reference</t>
   </si>
   <si>
-    <t xml:space="preserve">buitin:any</t>
-  </si>
-  <si>
     <t xml:space="preserve">Legacy GUID (Globally Unique Identifier) reference</t>
   </si>
   <si>
-    <t xml:space="preserve">builtin:any</t>
-  </si>
-  <si>
     <t xml:space="preserve">Location in Asset Hierarchy</t>
   </si>
   <si>
-    <t xml:space="preserve">builtin:floc</t>
+    <t xml:space="preserve">floc</t>
   </si>
   <si>
     <t xml:space="preserve">ABB01-SSS-SFS-HSE-SYS02</t>
@@ -280,6 +286,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -375,19 +382,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D65"/>
+  <dimension ref="A1:E65"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A48" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G71" activeCellId="0" sqref="G71"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="42.28"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="31.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="26.3"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="26.31"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -403,412 +410,448 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>15</v>
+        <v>7</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D55" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
+      </c>
+      <c r="E55" s="0" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>6</v>
+        <v>6</v>
+      </c>
+      <c r="C57" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>70</v>
+        <v>7</v>
+      </c>
+      <c r="D58" s="0" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="B59" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C59" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D59" s="0" t="s">
         <v>71</v>
-      </c>
-      <c r="B59" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C59" s="0" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C60" s="2" t="s">
-        <v>74</v>
+        <v>6</v>
+      </c>
+      <c r="C60" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C61" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D61" s="0" t="s">
-        <v>77</v>
+        <v>6</v>
+      </c>
+      <c r="C61" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E61" s="0" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>6</v>
+        <v>6</v>
+      </c>
+      <c r="C62" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>74</v>
+        <v>7</v>
+      </c>
+      <c r="D63" s="0" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>74</v>
+        <v>7</v>
+      </c>
+      <c r="D64" s="0" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>